<commit_message>
Changed titles of roles
</commit_message>
<xml_diff>
--- a/Roles_AMDR.xlsx
+++ b/Roles_AMDR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denniszomar/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E128AC5-5314-A249-8244-E3FEC084CC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E8C294-3515-6543-80F0-E84F331CB9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{6CB77485-1796-3F4C-8081-31D6D3A7341D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Title</t>
   </si>
@@ -65,16 +65,19 @@
     <t>CSEDS</t>
   </si>
   <si>
-    <t>Deputy Integration Lead</t>
-  </si>
-  <si>
-    <t>Test Director</t>
-  </si>
-  <si>
-    <t>Integration Lead / Site Lead</t>
-  </si>
-  <si>
-    <t>Integration Lead</t>
+    <t>ARDEL Deputy Integration Lead</t>
+  </si>
+  <si>
+    <t>AMDR Test Director</t>
+  </si>
+  <si>
+    <t>ARDEL Integration Lead / Site Lead</t>
+  </si>
+  <si>
+    <t>CSEDS Integration Lead</t>
+  </si>
+  <si>
+    <t>AMDR Integration Lead</t>
   </si>
 </sst>
 </file>
@@ -430,12 +433,12 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -542,7 +545,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>

</xml_diff>